<commit_message>
na poczatek dnia pisania we wtorek
</commit_message>
<xml_diff>
--- a/tabela1.xlsx
+++ b/tabela1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t xml:space="preserve">Lp.</t>
   </si>
@@ -32,6 +32,15 @@
   </si>
   <si>
     <t xml:space="preserve">okres T=t/k [s]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SREDNIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BLAD</t>
   </si>
 </sst>
 </file>
@@ -136,19 +145,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.11224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.8214285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.7448979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.5612244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.05102040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -313,6 +322,33 @@
       <c r="D11" s="1" t="n">
         <f aca="false">$C11/$B11</f>
         <v>1.25575</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <f aca="false">AVERAGE(D2:D11)</f>
+        <v>1.2493075</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <f aca="false">(4*3.141*3.141*0.396)/(D12*D12)</f>
+        <v>10.012726550512</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <f aca="false">(D13-9.81)/9.81 * 100</f>
+        <v>2.06652956689077</v>
       </c>
     </row>
   </sheetData>

</xml_diff>